<commit_message>
Se agregan boton izq y botón derecha al pinout.
</commit_message>
<xml_diff>
--- a/Pinout.xlsx
+++ b/Pinout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Juan\Documents\GitHub\Parcial1TD3.FRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC09BB93-9A9D-41AB-8179-20B976479FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C48C64-A50A-4D19-ABF2-F4B2E1099BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{0C0055F4-DE79-4D45-A8F8-1A9A34018993}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0C0055F4-DE79-4D45-A8F8-1A9A34018993}"/>
   </bookViews>
   <sheets>
     <sheet name="PINES LPC1769" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="159">
   <si>
     <t>Pin</t>
   </si>
@@ -507,6 +507,12 @@
   </si>
   <si>
     <t>RPM</t>
+  </si>
+  <si>
+    <t>Botón Izq</t>
+  </si>
+  <si>
+    <t>Botón Der</t>
   </si>
 </sst>
 </file>
@@ -1741,8 +1747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8702FAE-76D2-45C0-ADC7-52792CED1F3C}">
   <dimension ref="B2:Q29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2542,6 +2548,9 @@
       <c r="F27" t="s">
         <v>117</v>
       </c>
+      <c r="H27" t="s">
+        <v>157</v>
+      </c>
       <c r="K27">
         <v>52</v>
       </c>
@@ -2573,6 +2582,9 @@
       </c>
       <c r="F28" t="s">
         <v>119</v>
+      </c>
+      <c r="H28" t="s">
+        <v>158</v>
       </c>
       <c r="K28">
         <v>53</v>
@@ -2622,7 +2634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFAC58D6-936A-42BA-8DE0-F9E3DE8AC18A}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
agrego boton1 y 2
</commit_message>
<xml_diff>
--- a/Pinout.xlsx
+++ b/Pinout.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Juan\Documents\GitHub\Parcial1TD3.FRA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Diego\Documents\github\Parcial1TD3.FRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C48C64-A50A-4D19-ABF2-F4B2E1099BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2317789A-F7A9-4B34-BB57-0E8A02D7F9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0C0055F4-DE79-4D45-A8F8-1A9A34018993}"/>
   </bookViews>
@@ -1748,7 +1748,7 @@
   <dimension ref="B2:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>